<commit_message>
leetcode: #15 3Sum solution
</commit_message>
<xml_diff>
--- a/doc/Leetcode 75 Questions (NeetCode on yt).xlsx
+++ b/doc/Leetcode 75 Questions (NeetCode on yt).xlsx
@@ -2,13 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileSharing readOnlyRecommended="1"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\workspace\java\leetcode\leetcode\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DC7FC6B-D1E5-42D5-9631-B6E76EE3A8CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1641DFA4-A56B-4894-B356-767BC5A695E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1500,7 +1501,7 @@
   <dimension ref="A1:E1002"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>

</xml_diff>